<commit_message>
Examined all sex ratio data
</commit_message>
<xml_diff>
--- a/output/stats-results.xlsx
+++ b/output/stats-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles.Burks\MyGit\ms-now-ppo-kairomone-2017-2yr\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{209DDF60-249E-44C3-882F-40E6BE8B5CDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8ECCA6F2-9512-46DD-BD5F-8F51A025CD4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15468" yWindow="-108" windowWidth="15576" windowHeight="11904"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Experiment</t>
   </si>
@@ -121,6 +121,9 @@
     <t>F = 34.87, df = 6,42; P &lt; 0.001</t>
   </si>
   <si>
+    <t>y18_sex_ratios</t>
+  </si>
+  <si>
     <t>script6</t>
   </si>
   <si>
@@ -130,13 +133,13 @@
     <t>PROC CORR, PROC UNIVARIATE</t>
   </si>
   <si>
-    <t>y18_sex_ratios</t>
-  </si>
-  <si>
     <t>N = 5, rho = -0.9, P = 0.037</t>
   </si>
   <si>
-    <t>Mixed model ANOVA</t>
+    <t>GLMM with binomial dist</t>
+  </si>
+  <si>
+    <t>F = 6.43, df = 3, 19; P = 0.0034</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F12" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
   <tableColumns count="6">
     <tableColumn id="1" name="Experiment" dataDxfId="0"/>
     <tableColumn id="2" name="Part"/>
@@ -998,16 +1001,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
@@ -1118,7 +1122,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -1136,7 +1140,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -1226,19 +1230,33 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 2018 lures test
</commit_message>
<xml_diff>
--- a/output/stats-results.xlsx
+++ b/output/stats-results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles.Burks\MyGit\ms-now-ppo-kairomone-2017-2yr\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8ECCA6F2-9512-46DD-BD5F-8F51A025CD4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEC5E7-5AAD-46CC-B377-505EF9B59921}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15468" yWindow="-108" windowWidth="15576" windowHeight="11904"/>
+    <workbookView xWindow="5316" yWindow="1584" windowWidth="12888" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats-results" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>F = 20.11, df = 4, 27; P &lt; 0.001</t>
   </si>
   <si>
-    <t>F = 7.89, df = 4, 25; P &lt; 0.001</t>
-  </si>
-  <si>
     <t>F = 16.01, df = 4,27; P &lt; 0.001</t>
   </si>
   <si>
@@ -140,12 +137,15 @@
   </si>
   <si>
     <t>F = 6.43, df = 3, 19; P = 0.0034</t>
+  </si>
+  <si>
+    <t>F = 10.86, df = 4, 25; P &lt; 0.001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,14 +691,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Experiment" dataDxfId="0"/>
-    <tableColumn id="2" name="Part"/>
-    <tableColumn id="3" name="Script"/>
-    <tableColumn id="4" name="Procedure"/>
-    <tableColumn id="5" name="How"/>
-    <tableColumn id="6" name="Result"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Experiment" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Script"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Procedure"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="How"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Result"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1000,11 +1000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,7 +1146,7 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1164,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1172,10 +1172,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1184,16 +1184,16 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -1202,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1210,10 +1210,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1222,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1230,33 +1230,33 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>